<commit_message>
Corrected T° MSB formula
Changed formula in cell S7
From =(BIN2DEC(O7)*6.4) – 20
To =(BIN2DEC(R7)*6.4) – 20
</commit_message>
<xml_diff>
--- a/sensitv2_decoder_v0.1.xlsx
+++ b/sensitv2_decoder_v0.1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GS/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GS/Documents/sensitv2-decoder/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Uplink" sheetId="1" r:id="rId1"/>
@@ -500,9 +500,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -511,6 +508,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -794,7 +794,7 @@
   <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,7 +816,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="31" t="s">
         <v>34</v>
       </c>
       <c r="C1">
@@ -833,7 +833,7 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B2" s="26"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="12" t="s">
         <v>27</v>
       </c>
@@ -1046,8 +1046,8 @@
         <v>0110</v>
       </c>
       <c r="S7" s="24">
-        <f>(BIN2DEC(O7)*6.4) - 20</f>
-        <v>5.6000000000000014</v>
+        <f>(BIN2DEC(R7)*6.4) - 20</f>
+        <v>18.400000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
       <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="29">
         <v>-20</v>
       </c>
       <c r="E3" s="2" t="str">
@@ -1261,7 +1261,7 @@
       <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <v>107</v>
       </c>
       <c r="E4" s="2" t="str">
@@ -1297,7 +1297,7 @@
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="2" t="str">
@@ -1346,7 +1346,7 @@
       <c r="B8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="30">
         <v>0</v>
       </c>
       <c r="D8" s="25">
@@ -1362,7 +1362,7 @@
       <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="str">
@@ -1374,7 +1374,7 @@
       <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="30">
         <v>39</v>
       </c>
       <c r="D10" s="25">
@@ -1390,7 +1390,7 @@
       <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>2014</v>
       </c>
       <c r="E11" s="2" t="str">
@@ -1407,7 +1407,7 @@
       <c r="B14" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>61</v>
       </c>
       <c r="E14" s="2" t="str">
@@ -1424,7 +1424,7 @@
       <c r="B17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="30" t="s">
         <v>68</v>
       </c>
       <c r="E17" s="2" t="str">
@@ -1441,7 +1441,7 @@
       <c r="B20" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>77</v>
       </c>
       <c r="E20" s="2">
@@ -1523,7 +1523,7 @@
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -1537,10 +1537,10 @@
       <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="28" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1551,10 +1551,10 @@
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="28" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1565,10 +1565,10 @@
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="28" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1579,12 +1579,12 @@
       <c r="B7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1592,10 +1592,10 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="28">
-        <v>1</v>
-      </c>
-      <c r="F9" s="29" t="s">
+      <c r="E9" s="27">
+        <v>1</v>
+      </c>
+      <c r="F9" s="28" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1606,10 +1606,10 @@
       <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <v>8</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="28" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1620,10 +1620,10 @@
       <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="27">
         <v>64</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="28" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1634,10 +1634,10 @@
       <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="27">
         <v>2014</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="28" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1668,10 +1668,10 @@
       <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="28" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1682,10 +1682,10 @@
       <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="28" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1696,10 +1696,10 @@
       <c r="B18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="28" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1710,20 +1710,20 @@
       <c r="B19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="28" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1731,8 +1731,8 @@
       <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
@@ -1741,7 +1741,7 @@
       <c r="B22" s="11">
         <v>1</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1755,7 +1755,7 @@
       <c r="E23" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="26" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1783,7 +1783,7 @@
       <c r="E25" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="28" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>